<commit_message>
remove html br line breaks from case rule source
</commit_message>
<xml_diff>
--- a/lib/assets/rules.xlsx
+++ b/lib/assets/rules.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25711"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elnaz/Documents/dev/policeboard/lib/assets/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="11020" windowWidth="38400" windowHeight="10580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="11025" windowWidth="38400" windowHeight="10575" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="rules.csv" sheetId="1" r:id="rId1"/>
@@ -201,72 +196,43 @@
     <t xml:space="preserve">Failure to adequately secure and care for Department property. </t>
   </si>
   <si>
-    <r>
-      <t>Engaging in any public statements, interviews, activity, deliberation or discussion pertaining to the Police Department which reasonably can be foreseen to impair the discipline, efficiency, public service, or public confidence in the Department or its personnel by:  
-&lt;br/&gt;&lt;br/&gt;(a) false statements, or reckless, unsupported accusations. 
-&lt;br/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;br/&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(b) the use of defamatory language, abusive language, invective or epithets. </t>
-    </r>
+    <t xml:space="preserve">This Rule includes all incompetent and inefficient action on the part of any member and all failure to act when any policy, goal, rule, regulation, order, directive or rank would require positive action. </t>
   </si>
   <si>
     <t xml:space="preserve">A. Engaging directly or indirectly in the ownership, maintenance, or operation of a tavern or retail liquor establishment. 
-&lt;br/&gt;&lt;br/&gt;B. Engaging directly or indirectly in the ownership or leasing of a taxicab.  
-&lt;br/&gt;&lt;br/&gt;(Adopted by the Police Board 8 November 1979) </t>
+B. Engaging directly or indirectly in the ownership or leasing of a taxicab.  
+(Adopted by the Police Board 8 November 1979) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engaging in any public statements, interviews, activity, deliberation or discussion pertaining to the Police Department which reasonably can be foreseen to impair the discipline, efficiency, public service, or public confidence in the Department or its personnel by:  
+(a) false statements, or reckless, unsupported accusations. 
+(b) the use of defamatory language, abusive language, invective or epithets. </t>
   </si>
   <si>
     <t xml:space="preserve">A. Failure to testify or give evidence before any grand jury, coroner's inquest or court of law or before any governmental, administrative, or investigative agency (city, state or federal) when properly called upon to do so, and when there is no properly asserted constitutional privilege, or when immunity from prosecution has been granted. 
-&lt;br/&gt;&lt;br/&gt;B. Failure to cooperate when called to give evidence or statements by any investigative branch or superior officer of the Chicago Police Department or the Police Board when the evidence or statements sought relate specifically, directly and narrowly to the performance of his official duties.  If the member properly asserts a constitutional privilege, he will be required to cooperate if advised that by law any evidence or statements given by him cannot be used against him in a subsequent criminal prosecution. 
-&lt;br/&gt;&lt;br/&gt;(Effective 1 January 1975) </t>
+B. Failure to cooperate when called to give evidence or statements by any investigative branch or superior officer of the Chicago Police Department or the Police Board when the evidence or statements sought relate specifically, directly and narrowly to the performance of his official duties.  If the member properly asserts a constitutional privilege, he will be required to cooperate if advised that by law any evidence or statements given by him cannot be used against him in a subsequent criminal prosecution. 
+(Effective 1 January 1975) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seeking or soliciting contributions of any kind from anyone, by any means, for any purpose, under any circumstances, including collections for charitable purposes by any member or his agent, group of members or their agents, and including any sale or solicitation by any member or his agent, group of members or their agents, of advertising for any police journal, magazine or other publication identified with the Chicago Police Department or any association of its members, except as specifically authorized by resolution of the Police Board. 
+The members shall be subject to disciplinary action for any violation of this provision by his agent.  The officers, directors, or trustees of any association identified with members of the Chicago Police Pepartment shall be subject to disciplinary action for any violation of this provision made on behalf of the association by any member thereof or agents. These provisions do not apply to the solicitation of police personnel by police associations for memberships or dues. </t>
   </si>
   <si>
     <t xml:space="preserve">A. Joining or retaining membership in, or soliciting other members to join any labor organization whose membership is not exclusively limited to full time law enforcement officers.  It is provided that this Rule will not apply to civilian members nor to membership in any labor organization in connection with, and relating solely to, approved secondary employment of sworn officers. 
-&lt;br/&gt;&lt;br/&gt;B. Joining or retention of membership by supervisory personnel in any labor organization, whose membership is composed of rank and file members of the Department, and whose purpose is to represent its members concerning wages, hours, and working conditions.  It is provided that this Rule will not apply to the joining or retention of membership with rank and file members of the Department in organizations whose primary purpose is social, religious, ethnic or racial. </t>
+B. Joining or retention of membership by supervisory personnel in any labor organization, whose membership is composed of rank and file members of the Department, and whose purpose is to represent its members concerning wages, hours, and working conditions.  It is provided that this Rule will not apply to the joining or retention of membership with rank and file members of the Department in organizations whose primary purpose is social, religious, ethnic or racial. </t>
   </si>
   <si>
     <t xml:space="preserve"> A. Labor-management disputes frequently develop into situations requiring the presence and/or action of law enforcement officers to ensure that the rights of both labor and management are not violated by criminal acts.  Law enforcement's posture in these disputes must be one of strict and absolute neutrality and impartiality.  The policy of absolute neutrality and impartiality is seriously threatened and potentially undermined if the labor organization or union involved in the dispute is in any way associated with the representation of law enforcement officers of the law enforcement profession.  Membership in a labor union as defined above creates a potential conflict of interest which conflict is specifically prohibited by the Law Enforcement Code of Ethics to which we all adhere and which could lead to acts or failures to act contrary to law. 
-&lt;br/&gt;&lt;br/&gt;B. Supervisory personnel means any sworn member of the rank of sergeant and above.  Due to the growing activities of police labor organizations in regard to wages, hours, and working conditions, the membership of supervisory personnel who are charged with 
+B. Supervisory personnel means any sworn member of the rank of sergeant and above.  Due to the growing activities of police labor organizations in regard to wages, hours, and working conditions, the membership of supervisory personnel who are charged with 
 supervising rank and file members in regard to wages, hours, and working conditions would be present a conflict of interest. 
-&lt;br/&gt;&lt;br/&gt;(Effective 19 January 1976) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This Rule includes all incompetent and inefficient action on the part of any member and all failure to act when any policy, goal, rule, regulation, order, directive or rank would require positive action. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seeking or soliciting contributions of any kind from anyone, by any means, for any purpose, under any circumstances, including collections for charitable purposes by any member or his agent, group of members or their agents, and including any sale or solicitation by any member or his agent, group of members or their agents, of advertising for any police journal, magazine or other publication identified with the Chicago Police Department or any association of its members, except as specifically authorized by resolution of the Police Board. 
-&lt;br/&gt;&lt;br/&gt;The members shall be subject to disciplinary action for any violation of this provision by his agent.  The officers, directors, or trustees of any association identified with members of the Chicago Police Pepartment shall be subject to disciplinary action for any violation of this provision made on behalf of the association by any member thereof or agents. &lt;br/&gt;&lt;br/&gt;These provisions do not apply to the solicitation of police personnel by police associations for memberships or dues. </t>
+(Effective 19 January 1976) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -570,7 +536,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -580,17 +546,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="255.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -601,7 +567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -609,7 +575,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -620,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -631,7 +597,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -639,7 +605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -647,7 +613,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -658,7 +624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -666,7 +632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -674,7 +640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -685,7 +651,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -693,7 +659,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -701,10 +667,10 @@
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -712,7 +678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -720,7 +686,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -728,7 +694,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -736,7 +702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -744,7 +710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -752,7 +718,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -760,7 +726,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -768,7 +734,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -776,7 +742,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -784,7 +750,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -792,7 +758,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -800,7 +766,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -808,7 +774,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -816,7 +782,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -824,7 +790,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -832,7 +798,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -840,7 +806,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -848,7 +814,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -856,7 +822,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -867,15 +833,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -883,7 +849,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -891,7 +857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -899,7 +865,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -907,7 +873,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -915,7 +881,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -923,7 +889,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -931,7 +897,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -939,7 +905,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -947,7 +913,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -955,7 +921,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -963,7 +929,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -971,7 +937,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -979,7 +945,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -987,7 +953,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -995,7 +961,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1003,7 +969,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1011,7 +977,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1019,23 +985,23 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1043,18 +1009,18 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="2" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" s="2" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>

</xml_diff>